<commit_message>
Some doc stuff mostly
</commit_message>
<xml_diff>
--- a/docs/roboticAntStatus.xlsx
+++ b/docs/roboticAntStatus.xlsx
@@ -786,8 +786,8 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixing some capacitive sensor stuff
</commit_message>
<xml_diff>
--- a/docs/roboticAntStatus.xlsx
+++ b/docs/roboticAntStatus.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
   <si>
     <t>Robot Alpha</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Changed which set of pins were connected to the Gripper Servo and now things seem to be working fine. I also replaced the battery pack and Delta is more agile now. Also calibrated the IMU.</t>
+  </si>
+  <si>
+    <t>The lower left hall effect sensor wires are broken. Robot still functional. Moved the 5V for Pixy from the PDB to the Arduino 5V pin. Hoping that this line is better regulated, and will prevent the Pixy from wiping the memory so frequently.</t>
   </si>
 </sst>
 </file>
@@ -783,11 +786,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,6 +1220,26 @@
         <v>112</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
+        <v>42708</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Formatting stuff relevant to lorenz runs and some documentation stuff
</commit_message>
<xml_diff>
--- a/docs/roboticAntStatus.xlsx
+++ b/docs/roboticAntStatus.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="124">
   <si>
     <t>Robot Alpha</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>Fixed disconnected wires. Note that this may be a recurring issue on this robot.</t>
+  </si>
+  <si>
+    <t>May not need to replace IMU now that a new calibration technique has been implemented.</t>
   </si>
 </sst>
 </file>
@@ -827,11 +830,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,6 +1445,26 @@
       </c>
       <c r="F30" s="2" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
+        <v>42738</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More PID control stuff
Also added some camera stuff back in for detecting the color green
</commit_message>
<xml_diff>
--- a/docs/roboticAntStatus.xlsx
+++ b/docs/roboticAntStatus.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
   <si>
     <t>Robot Alpha</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>May not need to replace IMU now that a new calibration technique has been implemented.</t>
+  </si>
+  <si>
+    <t>Need to print out another motor mount bracket.</t>
   </si>
 </sst>
 </file>
@@ -830,11 +833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,6 +1468,26 @@
       </c>
       <c r="F31" s="3" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>42742</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated goingOut implementation and tuned caps
</commit_message>
<xml_diff>
--- a/docs/roboticAntStatus.xlsx
+++ b/docs/roboticAntStatus.xlsx
@@ -836,8 +836,8 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Transitioning away from the Fio
</commit_message>
<xml_diff>
--- a/docs/roboticAntStatus.xlsx
+++ b/docs/roboticAntStatus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="12120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Status" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="138">
   <si>
     <t>Robot Alpha</t>
   </si>
@@ -431,6 +431,15 @@
   </si>
   <si>
     <t>Fixed gripper</t>
+  </si>
+  <si>
+    <t>Check the current sensor.</t>
+  </si>
+  <si>
+    <t>I can make this reset by stalling the motors.</t>
+  </si>
+  <si>
+    <t>Pixy is now on Due 5v.</t>
   </si>
 </sst>
 </file>
@@ -863,11 +872,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,6 +1667,26 @@
       </c>
       <c r="F39" s="3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="15">
+        <v>42773</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -29755,8 +29784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="100.7109375" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>